<commit_message>
Fix some error in slide 16
</commit_message>
<xml_diff>
--- a/Excel动手实验室 - 材料/09 - 数据排序和筛选.xlsx
+++ b/Excel动手实验室 - 材料/09 - 数据排序和筛选.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="8100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="347" windowWidth="18434" windowHeight="8097"/>
   </bookViews>
   <sheets>
     <sheet name="排序和筛选" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -152,7 +152,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -160,7 +160,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -168,14 +168,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -184,7 +184,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -553,13 +553,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="8.875" customWidth="1"/>
-    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -746,15 +746,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -927,14 +927,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="8.875" customWidth="1"/>
-    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>